<commit_message>
correçâo semana 4 grupo 3 ELET3
</commit_message>
<xml_diff>
--- a/d-3/4Semana/1992-2005_ResultadosFinais_04_03.xlsx
+++ b/d-3/4Semana/1992-2005_ResultadosFinais_04_03.xlsx
@@ -1,32 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\eng-eco\d-3\4Semana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20C5AAAF-77C5-48E0-BE76-0250409EC89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C818B1F5-190B-423E-AA99-3C6134AB91C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1992-2005" sheetId="1" r:id="rId1"/>
     <sheet name="RESULTADOS FINAIS " sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>DELL</author>
   </authors>
   <commentList>
-    <comment ref="F2" authorId="0" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -79,6 +79,21 @@
         </r>
       </text>
     </comment>
+    <comment ref="K15" authorId="0" shapeId="0" xr:uid="{07F1671D-949A-4B06-AED2-C7CF55FA17C7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Todas as ações acumuladas foram vendidas no ano de 2023
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -596,7 +611,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
@@ -771,7 +786,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -981,8 +996,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1191,6 +1212,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1237,10 +1313,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1321,6 +1396,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="16" fillId="37" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="38" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="16" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1681,1956 +1774,1969 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L352"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M17" sqref="K4:M17"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
     <col min="7" max="7" width="32" customWidth="1"/>
     <col min="8" max="8" width="34.7109375" customWidth="1"/>
     <col min="11" max="11" width="32.7109375" customWidth="1"/>
-    <col min="12" max="12" width="29.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="29.85546875" style="3" customWidth="1"/>
     <col min="13" max="13" width="29.140625" customWidth="1"/>
     <col min="14" max="14" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+      <c r="A2" s="16">
         <v>1992</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18">
         <v>0.23</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="16">
         <v>1500</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="20">
+      <c r="E2" s="16"/>
+      <c r="F2" s="19">
         <v>71681</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
+      <c r="A3" s="16">
         <v>1993</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="21">
+      <c r="B3" s="17"/>
+      <c r="C3" s="20">
         <v>0.31</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <v>1500</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="20">
+      <c r="E3" s="16"/>
+      <c r="F3" s="19">
         <v>1949630</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>1.48</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <f>(1500+194963)/B4</f>
         <v>132745.27027027027</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="K4" t="s">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2.33</v>
+      </c>
+      <c r="E5" s="4">
+        <f>1500/B5</f>
+        <v>643.77682403433471</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="K5" s="41" t="s">
         <v>167</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L5" s="42">
         <f>1500*360</f>
         <v>540000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3">
-        <v>2.33</v>
-      </c>
-      <c r="E5" s="5">
-        <f>1500/B5</f>
-        <v>643.77682403433471</v>
-      </c>
-      <c r="H5" s="1"/>
-    </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>2.6</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <f t="shared" ref="E6:E14" si="0">1500/B6</f>
         <v>576.92307692307691</v>
       </c>
       <c r="H6" s="1"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="43"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>3.43</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <f t="shared" si="0"/>
         <v>437.31778425655972</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="K7" t="s">
+      <c r="K7" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="43">
         <f>H14*B135</f>
         <v>3467322.2745452328</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>5.47</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <f t="shared" si="0"/>
         <v>274.22303473491775</v>
       </c>
       <c r="H8" s="1"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="43"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>6.05</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <f t="shared" si="0"/>
         <v>247.93388429752068</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="22" t="s">
         <v>161</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="K9" t="s">
+      <c r="K9" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="L9" s="4">
-        <v>88051</v>
+      <c r="L9" s="43">
+        <f>75000*10.93</f>
+        <v>819750</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>9.31</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <f t="shared" si="0"/>
         <v>161.11707841031148</v>
       </c>
       <c r="H10" s="1"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="45"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>9.4700000000000006</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <f t="shared" si="0"/>
         <v>158.39493136219639</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="L11" s="4">
-        <v>271798</v>
+      <c r="L11" s="43">
+        <f>129000*83.9</f>
+        <v>10823100</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>8.42</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <f t="shared" si="0"/>
         <v>178.14726840855107</v>
       </c>
+      <c r="K12" s="44"/>
+      <c r="L12" s="43"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>7.63</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <f t="shared" si="0"/>
         <v>196.5923984272608</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <f>1500*156</f>
         <v>234000</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="L13" s="4">
-        <v>282701</v>
+      <c r="L13" s="43">
+        <f>(222*263)*5.29</f>
+        <v>308861.94</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>7.65</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <f t="shared" si="0"/>
         <v>196.07843137254901</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="7">
         <f>SUM(E4:E135)</f>
         <v>399461.09153746924</v>
       </c>
+      <c r="K14" s="38"/>
+      <c r="L14" s="39"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>7.24</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <f>(1500+194963)/B15</f>
         <v>27135.773480662981</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="37">
         <f>SUM(L7:L13)</f>
-        <v>4109872.2745452328</v>
+        <v>15419034.214545233</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>4.91</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <f>1500/B16</f>
         <v>305.49898167006108</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G16" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="9" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>4.53</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <f t="shared" ref="E17:E26" si="1">1500/B17</f>
         <v>331.1258278145695</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="11">
         <f>-H13</f>
         <v>-234000</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="2">
         <v>6.45</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <f t="shared" si="1"/>
         <v>232.55813953488371</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="12">
         <f>F2</f>
         <v>71681</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>6.45</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <f t="shared" si="1"/>
         <v>232.55813953488371</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="12">
         <f>F3</f>
         <v>1949630</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>6.14</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <f t="shared" si="1"/>
         <v>244.29967426710098</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="12">
         <f>SUM(E4:E14)*B14</f>
         <v>1038990.6786161064</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="2">
         <v>6.45</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <f t="shared" si="1"/>
         <v>232.55813953488371</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="G21" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="12">
         <f>SUM(E15:E26)*B26</f>
         <v>200472.65518851465</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>6.73</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <f t="shared" si="1"/>
         <v>222.88261515601781</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="H22" s="13">
+      <c r="H22" s="12">
         <f>SUM(E27:E38)*B38</f>
         <v>267107.80052104406</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="2">
         <v>7.53</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <f t="shared" si="1"/>
         <v>199.203187250996</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="H23" s="13">
+      <c r="H23" s="12">
         <f>SUM(E39:E50)*B50</f>
         <v>273529.11194876162</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="2">
         <v>6.99</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <f t="shared" si="1"/>
         <v>214.59227467811158</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="H24" s="13">
+      <c r="H24" s="12">
         <f>SUM(E51:E62)*B62</f>
         <v>95473.051236213229</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="2">
         <v>7.01</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <f t="shared" si="1"/>
         <v>213.98002853067047</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="H25" s="13">
+      <c r="H25" s="12">
         <f>SUM(E63:E74)*B74</f>
         <v>330161.4636976436</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="2">
         <v>6.73</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <f t="shared" si="1"/>
         <v>222.88261515601781</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="12">
         <f>SUM(E75:E86)*B86</f>
         <v>238678.71047788206</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="2">
         <v>7.63</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="4">
         <f>(1500+194963)/B27</f>
         <v>25748.754914809961</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="12">
         <f>SUM(E87:E98)*B98</f>
         <v>172352.37673575454</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="2">
         <v>6.96</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="4">
         <f>1500/B28</f>
         <v>215.51724137931035</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="12">
         <f>SUM(E99:E110)*B110</f>
         <v>143817.81730876505</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="2">
         <v>6.6</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="4">
         <f t="shared" ref="E29:E92" si="2">1500/B29</f>
         <v>227.27272727272728</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="H29" s="13">
+      <c r="H29" s="12">
         <f>SUM(E111:E122)*B122</f>
         <v>524699.18573213066</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="2">
         <v>6.12</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="4">
         <f t="shared" si="2"/>
         <v>245.09803921568627</v>
       </c>
-      <c r="G30" s="11" t="s">
+      <c r="G30" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="H30" s="13">
+      <c r="H30" s="12">
         <f>SUM(E46:E57)*B57</f>
         <v>156702.92010469624</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="2">
         <v>6.22</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="4">
         <f t="shared" si="2"/>
         <v>241.15755627009648</v>
       </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="H31" s="13">
+      <c r="H31" s="12">
         <f>SUM(E123:E135)*B135</f>
         <v>206605.22652710721</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="2">
         <v>6.91</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="4">
         <f t="shared" si="2"/>
         <v>217.07670043415339</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="2">
         <v>7.17</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="4">
         <f t="shared" si="2"/>
         <v>209.20502092050211</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <v>6.91</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="4">
         <f t="shared" si="2"/>
         <v>217.07670043415339</v>
       </c>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="2">
         <v>6.89</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="4">
         <f t="shared" si="2"/>
         <v>217.7068214804064</v>
       </c>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="2">
         <v>8.17</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="4">
         <f t="shared" si="2"/>
         <v>183.5985312117503</v>
       </c>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="2">
         <v>8.4499999999999993</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="4">
         <f t="shared" si="2"/>
         <v>177.51479289940829</v>
       </c>
-      <c r="G37" s="9" t="s">
+      <c r="G37" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="H37" s="14">
+      <c r="H37" s="13">
         <v>0.2</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="2">
         <v>9.52</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="4">
         <f t="shared" si="2"/>
         <v>157.56302521008405</v>
       </c>
-      <c r="G38" s="9" t="s">
+      <c r="G38" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="H38" s="15">
+      <c r="H38" s="14">
         <f>NPV(H37,H18:H31)+H17</f>
         <v>2363004.854910404</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="2">
         <v>10.93</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="4">
         <f>(1500+194963)/B39</f>
         <v>17974.65690759378</v>
       </c>
-      <c r="G39" s="9" t="s">
+      <c r="G39" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="H39" s="14">
+      <c r="H39" s="13">
         <f>IRR(H17:H31)</f>
         <v>2.2883381974886525</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="2">
         <v>11.83</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="4">
         <f t="shared" si="2"/>
         <v>126.79628064243448</v>
       </c>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="2">
         <v>11.21</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="4">
         <f t="shared" si="2"/>
         <v>133.80909901873326</v>
       </c>
       <c r="H41" s="1"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="2">
         <v>12.31</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="4">
         <f t="shared" si="2"/>
         <v>121.85215272136475</v>
       </c>
       <c r="H42" s="1"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="2">
         <v>12.93</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="4">
         <f t="shared" si="2"/>
         <v>116.0092807424594</v>
       </c>
       <c r="H43" s="1"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="2">
         <v>15.41</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="4">
         <f t="shared" si="2"/>
         <v>97.339390006489296</v>
       </c>
       <c r="H44" s="1"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="2">
         <v>15.1</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="4">
         <f t="shared" si="2"/>
         <v>99.337748344370866</v>
       </c>
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="2">
         <v>11.9</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="4">
         <f t="shared" si="2"/>
         <v>126.05042016806722</v>
       </c>
       <c r="H46" s="1"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="2">
         <v>14.85</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="4">
         <f t="shared" si="2"/>
         <v>101.01010101010101</v>
       </c>
       <c r="H47" s="1"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="2">
         <v>11.39</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48" s="4">
         <f t="shared" si="2"/>
         <v>131.69446883230904</v>
       </c>
       <c r="H48" s="1"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="2">
         <v>13.05</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="4">
         <f t="shared" si="2"/>
         <v>114.94252873563218</v>
       </c>
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="2">
         <v>14.21</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="4">
         <f t="shared" si="2"/>
         <v>105.55946516537649</v>
       </c>
       <c r="H50" s="1"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="2">
         <v>12.42</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="4">
         <f>(1500+194963)/B51</f>
         <v>15818.276972624799</v>
       </c>
       <c r="H51" s="1"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B52" s="3">
+      <c r="B52" s="2">
         <v>13</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="4">
         <f t="shared" si="2"/>
         <v>115.38461538461539</v>
       </c>
       <c r="H52" s="1"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="3">
+      <c r="B53" s="2">
         <v>13.52</v>
       </c>
-      <c r="E53" s="5">
+      <c r="E53" s="4">
         <f t="shared" si="2"/>
         <v>110.94674556213018</v>
       </c>
       <c r="H53" s="1"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="3">
+      <c r="B54" s="2">
         <v>12.03</v>
       </c>
-      <c r="E54" s="5">
+      <c r="E54" s="4">
         <f t="shared" si="2"/>
         <v>124.68827930174564</v>
       </c>
       <c r="H54" s="1"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B55" s="3">
+      <c r="B55" s="2">
         <v>9.8000000000000007</v>
       </c>
-      <c r="E55" s="5">
+      <c r="E55" s="4">
         <f t="shared" si="2"/>
         <v>153.0612244897959</v>
       </c>
       <c r="H55" s="1"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B56" s="3">
+      <c r="B56" s="2">
         <v>8.6999999999999993</v>
       </c>
-      <c r="E56" s="5">
+      <c r="E56" s="4">
         <f t="shared" si="2"/>
         <v>172.41379310344828</v>
       </c>
       <c r="H56" s="1"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B57" s="3">
+      <c r="B57" s="2">
         <v>9.09</v>
       </c>
-      <c r="E57" s="5">
+      <c r="E57" s="4">
         <f t="shared" si="2"/>
         <v>165.01650165016503</v>
       </c>
       <c r="H57" s="1"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B58" s="3">
+      <c r="B58" s="2">
         <v>4.3</v>
       </c>
-      <c r="E58" s="5">
+      <c r="E58" s="4">
         <f t="shared" si="2"/>
         <v>348.83720930232562</v>
       </c>
       <c r="H58" s="1"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B59" s="3">
+      <c r="B59" s="2">
         <v>6.3</v>
       </c>
-      <c r="E59" s="5">
+      <c r="E59" s="4">
         <f t="shared" si="2"/>
         <v>238.0952380952381</v>
       </c>
       <c r="H59" s="1"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B60" s="3">
+      <c r="B60" s="2">
         <v>6.6</v>
       </c>
-      <c r="E60" s="5">
+      <c r="E60" s="4">
         <f t="shared" si="2"/>
         <v>227.27272727272728</v>
       </c>
       <c r="H60" s="1"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B61" s="3">
+      <c r="B61" s="2">
         <v>7.89</v>
       </c>
-      <c r="E61" s="5">
+      <c r="E61" s="4">
         <f t="shared" si="2"/>
         <v>190.11406844106466</v>
       </c>
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="3">
+      <c r="B62" s="2">
         <v>5.32</v>
       </c>
-      <c r="E62" s="5">
+      <c r="E62" s="4">
         <f t="shared" si="2"/>
         <v>281.95488721804509</v>
       </c>
       <c r="H62" s="1"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="3">
+      <c r="B63" s="2">
         <v>6.4</v>
       </c>
-      <c r="E63" s="5">
+      <c r="E63" s="4">
         <f>(1500+194963)/B63</f>
         <v>30697.34375</v>
       </c>
       <c r="H63" s="1"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B64" s="3">
+      <c r="B64" s="2">
         <v>6.91</v>
       </c>
-      <c r="E64" s="5">
+      <c r="E64" s="4">
         <f t="shared" si="2"/>
         <v>217.07670043415339</v>
       </c>
       <c r="H64" s="1"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B65" s="3">
+      <c r="B65" s="2">
         <v>8.57</v>
       </c>
-      <c r="E65" s="5">
+      <c r="E65" s="4">
         <f t="shared" si="2"/>
         <v>175.02917152858808</v>
       </c>
       <c r="H65" s="1"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B66" s="3">
+      <c r="B66" s="2">
         <v>8.68</v>
       </c>
-      <c r="E66" s="5">
+      <c r="E66" s="4">
         <f t="shared" si="2"/>
         <v>172.81105990783411</v>
       </c>
       <c r="H66" s="1"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="2">
         <v>9.06</v>
       </c>
-      <c r="E67" s="5">
+      <c r="E67" s="4">
         <f t="shared" si="2"/>
         <v>165.56291390728475</v>
       </c>
       <c r="H67" s="1"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B68" s="3">
+      <c r="B68" s="2">
         <v>8.5500000000000007</v>
       </c>
-      <c r="E68" s="5">
+      <c r="E68" s="4">
         <f t="shared" si="2"/>
         <v>175.43859649122805</v>
       </c>
       <c r="H68" s="1"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B69" s="3">
+      <c r="B69" s="2">
         <v>7.45</v>
       </c>
-      <c r="E69" s="5">
+      <c r="E69" s="4">
         <f t="shared" si="2"/>
         <v>201.34228187919462</v>
       </c>
       <c r="H69" s="1"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B70" s="3">
+      <c r="B70" s="2">
         <v>7.65</v>
       </c>
-      <c r="E70" s="5">
+      <c r="E70" s="4">
         <f t="shared" si="2"/>
         <v>196.07843137254901</v>
       </c>
       <c r="H70" s="1"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B71" s="3">
+      <c r="B71" s="2">
         <v>8.19</v>
       </c>
-      <c r="E71" s="5">
+      <c r="E71" s="4">
         <f t="shared" si="2"/>
         <v>183.15018315018315</v>
       </c>
       <c r="H71" s="1"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B72" s="3">
+      <c r="B72" s="2">
         <v>8.6</v>
       </c>
-      <c r="E72" s="5">
+      <c r="E72" s="4">
         <f t="shared" si="2"/>
         <v>174.41860465116281</v>
       </c>
       <c r="H72" s="1"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="2">
         <v>9.98</v>
       </c>
-      <c r="E73" s="5">
+      <c r="E73" s="4">
         <f t="shared" si="2"/>
         <v>150.30060120240481</v>
       </c>
       <c r="H73" s="1"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="2">
         <v>10.11</v>
       </c>
-      <c r="E74" s="5">
+      <c r="E74" s="4">
         <f t="shared" si="2"/>
         <v>148.36795252225519</v>
       </c>
       <c r="H74" s="1"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B75" s="3">
+      <c r="B75" s="2">
         <v>8.2200000000000006</v>
       </c>
-      <c r="E75" s="5">
+      <c r="E75" s="4">
         <f>(1500+194963)/B75</f>
         <v>23900.608272506081</v>
       </c>
       <c r="H75" s="1"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B76" s="3">
+      <c r="B76" s="2">
         <v>7.86</v>
       </c>
-      <c r="E76" s="5">
+      <c r="E76" s="4">
         <f t="shared" si="2"/>
         <v>190.83969465648855</v>
       </c>
       <c r="H76" s="1"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B77" s="3">
+      <c r="B77" s="2">
         <v>7.94</v>
       </c>
-      <c r="E77" s="5">
+      <c r="E77" s="4">
         <f t="shared" si="2"/>
         <v>188.91687657430731</v>
       </c>
       <c r="H77" s="1"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B78" s="3">
+      <c r="B78" s="2">
         <v>6.83</v>
       </c>
-      <c r="E78" s="5">
+      <c r="E78" s="4">
         <f t="shared" si="2"/>
         <v>219.61932650073206</v>
       </c>
       <c r="H78" s="1"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B79" s="3">
+      <c r="B79" s="2">
         <v>7.44</v>
       </c>
-      <c r="E79" s="5">
+      <c r="E79" s="4">
         <f t="shared" si="2"/>
         <v>201.61290322580643</v>
       </c>
       <c r="H79" s="1"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B80" s="3">
+      <c r="B80" s="2">
         <v>9.4700000000000006</v>
       </c>
-      <c r="E80" s="5">
+      <c r="E80" s="4">
         <f t="shared" si="2"/>
         <v>158.39493136219639</v>
       </c>
       <c r="H80" s="1"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B81" s="3">
+      <c r="B81" s="2">
         <v>10.11</v>
       </c>
-      <c r="E81" s="5">
+      <c r="E81" s="4">
         <f t="shared" si="2"/>
         <v>148.36795252225519</v>
       </c>
       <c r="H81" s="1"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B82" s="2">
         <v>8.73</v>
       </c>
-      <c r="E82" s="5">
+      <c r="E82" s="4">
         <f t="shared" si="2"/>
         <v>171.82130584192439</v>
       </c>
       <c r="H82" s="1"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B83" s="3">
+      <c r="B83" s="2">
         <v>9.19</v>
       </c>
-      <c r="E83" s="5">
+      <c r="E83" s="4">
         <f t="shared" si="2"/>
         <v>163.22089227421111</v>
       </c>
       <c r="H83" s="1"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B84" s="3">
+      <c r="B84" s="2">
         <v>8.68</v>
       </c>
-      <c r="E84" s="5">
+      <c r="E84" s="4">
         <f t="shared" si="2"/>
         <v>172.81105990783411</v>
       </c>
       <c r="H84" s="1"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B85" s="3">
+      <c r="B85" s="2">
         <v>8.32</v>
       </c>
-      <c r="E85" s="5">
+      <c r="E85" s="4">
         <f t="shared" si="2"/>
         <v>180.28846153846152</v>
       </c>
       <c r="H85" s="1"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B86" s="3">
+      <c r="B86" s="2">
         <v>9.23</v>
       </c>
-      <c r="E86" s="5">
+      <c r="E86" s="4">
         <f t="shared" si="2"/>
         <v>162.51354279523292</v>
       </c>
       <c r="H86" s="1"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B87" s="3">
+      <c r="B87" s="2">
         <v>10.7</v>
       </c>
-      <c r="E87" s="5">
+      <c r="E87" s="4">
         <f>(1500+194963)/B87</f>
         <v>18361.028037383177</v>
       </c>
       <c r="H87" s="1"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B88" s="2">
         <v>10.25</v>
       </c>
-      <c r="E88" s="5">
+      <c r="E88" s="4">
         <f t="shared" si="2"/>
         <v>146.34146341463415</v>
       </c>
       <c r="H88" s="1"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B89" s="3">
+      <c r="B89" s="2">
         <v>10.62</v>
       </c>
-      <c r="E89" s="5">
+      <c r="E89" s="4">
         <f t="shared" si="2"/>
         <v>141.24293785310735</v>
       </c>
       <c r="H89" s="1"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B90" s="3">
+      <c r="B90" s="2">
         <v>9.6</v>
       </c>
-      <c r="E90" s="5">
+      <c r="E90" s="4">
         <f t="shared" si="2"/>
         <v>156.25</v>
       </c>
       <c r="H90" s="1"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B91" s="3">
+      <c r="B91" s="2">
         <v>7.71</v>
       </c>
-      <c r="E91" s="5">
+      <c r="E91" s="4">
         <f t="shared" si="2"/>
         <v>194.55252918287937</v>
       </c>
       <c r="H91" s="1"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B92" s="3">
+      <c r="B92" s="2">
         <v>7.55</v>
       </c>
-      <c r="E92" s="5">
+      <c r="E92" s="4">
         <f t="shared" si="2"/>
         <v>198.67549668874173</v>
       </c>
       <c r="H92" s="1"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B93" s="3">
+      <c r="B93" s="2">
         <v>9.2200000000000006</v>
       </c>
-      <c r="E93" s="5">
+      <c r="E93" s="4">
         <f t="shared" ref="E93:E135" si="3">1500/B93</f>
         <v>162.68980477223425</v>
       </c>
       <c r="H93" s="1"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B94" s="3">
+      <c r="B94" s="2">
         <v>9.34</v>
       </c>
-      <c r="E94" s="5">
+      <c r="E94" s="4">
         <f t="shared" si="3"/>
         <v>160.59957173447538</v>
       </c>
       <c r="H94" s="1"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B95" s="3">
+      <c r="B95" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E95" s="5">
+      <c r="E95" s="4">
         <f t="shared" si="3"/>
         <v>182.92682926829269</v>
       </c>
       <c r="H95" s="1"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B96" s="3">
+      <c r="B96" s="2">
         <v>8.9600000000000009</v>
       </c>
-      <c r="E96" s="5">
+      <c r="E96" s="4">
         <f t="shared" si="3"/>
         <v>167.41071428571428</v>
       </c>
       <c r="H96" s="1"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B97" s="3">
+      <c r="B97" s="2">
         <v>8.27</v>
       </c>
-      <c r="E97" s="5">
+      <c r="E97" s="4">
         <f t="shared" si="3"/>
         <v>181.37847642079808</v>
       </c>
       <c r="H97" s="1"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B98" s="3">
+      <c r="B98" s="2">
         <v>8.52</v>
       </c>
-      <c r="E98" s="5">
+      <c r="E98" s="4">
         <f t="shared" si="3"/>
         <v>176.05633802816902</v>
       </c>
       <c r="H98" s="1"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B99" s="3">
+      <c r="B99" s="2">
         <v>9.26</v>
       </c>
-      <c r="E99" s="5">
+      <c r="E99" s="4">
         <f>(1500+194963)/B99</f>
         <v>21216.306695464362</v>
       </c>
       <c r="H99" s="1"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B100" s="3">
+      <c r="B100" s="2">
         <v>10.75</v>
       </c>
-      <c r="E100" s="5">
+      <c r="E100" s="4">
         <f t="shared" si="3"/>
         <v>139.53488372093022</v>
       </c>
       <c r="H100" s="1"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B101" s="3">
+      <c r="B101" s="2">
         <v>9.91</v>
       </c>
-      <c r="E101" s="5">
+      <c r="E101" s="4">
         <f t="shared" si="3"/>
         <v>151.3622603430878</v>
       </c>
       <c r="H101" s="1"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B102" s="3">
+      <c r="B102" s="2">
         <v>9.16</v>
       </c>
-      <c r="E102" s="5">
+      <c r="E102" s="4">
         <f t="shared" si="3"/>
         <v>163.75545851528383</v>
       </c>
       <c r="H102" s="1"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B103" s="3">
+      <c r="B103" s="2">
         <v>8.27</v>
       </c>
-      <c r="E103" s="5">
+      <c r="E103" s="4">
         <f t="shared" si="3"/>
         <v>181.37847642079808</v>
       </c>
       <c r="H103" s="1"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
+      <c r="A104" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B104" s="3">
+      <c r="B104" s="2">
         <v>7.52</v>
       </c>
-      <c r="E104" s="5">
+      <c r="E104" s="4">
         <f t="shared" si="3"/>
         <v>199.468085106383</v>
       </c>
       <c r="H104" s="1"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B105" s="3">
+      <c r="B105" s="2">
         <v>5.5</v>
       </c>
-      <c r="E105" s="5">
+      <c r="E105" s="4">
         <f t="shared" si="3"/>
         <v>272.72727272727275</v>
       </c>
       <c r="H105" s="1"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="3" t="s">
+      <c r="A106" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B106" s="3">
+      <c r="B106" s="2">
         <v>5.71</v>
       </c>
-      <c r="E106" s="5">
+      <c r="E106" s="4">
         <f t="shared" si="3"/>
         <v>262.69702276707528</v>
       </c>
       <c r="H106" s="1"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B107" s="3">
+      <c r="B107" s="2">
         <v>3.83</v>
       </c>
-      <c r="E107" s="5">
+      <c r="E107" s="4">
         <f t="shared" si="3"/>
         <v>391.64490861618799</v>
       </c>
       <c r="H107" s="1"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B108" s="3">
+      <c r="B108" s="2">
         <v>5.17</v>
       </c>
-      <c r="E108" s="5">
+      <c r="E108" s="4">
         <f t="shared" si="3"/>
         <v>290.13539651837527</v>
       </c>
       <c r="H108" s="1"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B109" s="3">
+      <c r="B109" s="2">
         <v>5.1100000000000003</v>
       </c>
-      <c r="E109" s="5">
+      <c r="E109" s="4">
         <f t="shared" si="3"/>
         <v>293.54207436399213</v>
       </c>
       <c r="H109" s="1"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
+      <c r="A110" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B110" s="3">
+      <c r="B110" s="2">
         <v>6.04</v>
       </c>
-      <c r="E110" s="5">
+      <c r="E110" s="4">
         <f t="shared" si="3"/>
         <v>248.34437086092714</v>
       </c>
       <c r="H110" s="1"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B111" s="3">
+      <c r="B111" s="2">
         <v>4.97</v>
       </c>
-      <c r="E111" s="5">
+      <c r="E111" s="4">
         <f>(1500+194963)/B111</f>
         <v>39529.778672032196</v>
       </c>
       <c r="H111" s="1"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
+      <c r="A112" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B112" s="3">
+      <c r="B112" s="2">
         <v>4.3</v>
       </c>
-      <c r="E112" s="5">
+      <c r="E112" s="4">
         <f t="shared" si="3"/>
         <v>348.83720930232562</v>
       </c>
       <c r="H112" s="1"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B113" s="3">
+      <c r="B113" s="2">
         <v>4.67</v>
       </c>
-      <c r="E113" s="5">
+      <c r="E113" s="4">
         <f t="shared" si="3"/>
         <v>321.19914346895075</v>
       </c>
       <c r="H113" s="1"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B114" s="3">
+      <c r="B114" s="2">
         <v>5.73</v>
       </c>
-      <c r="E114" s="5">
+      <c r="E114" s="4">
         <f t="shared" si="3"/>
         <v>261.78010471204186</v>
       </c>
       <c r="H114" s="1"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A115" s="3" t="s">
+      <c r="A115" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B115" s="3">
+      <c r="B115" s="2">
         <v>5.93</v>
       </c>
-      <c r="E115" s="5">
+      <c r="E115" s="4">
         <f t="shared" si="3"/>
         <v>252.95109612141653</v>
       </c>
       <c r="H115" s="1"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="3" t="s">
+      <c r="A116" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B116" s="3">
+      <c r="B116" s="2">
         <v>5.0599999999999996</v>
       </c>
-      <c r="E116" s="5">
+      <c r="E116" s="4">
         <f t="shared" si="3"/>
         <v>296.44268774703562</v>
       </c>
       <c r="H116" s="1"/>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A117" s="3" t="s">
+      <c r="A117" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B117" s="3">
+      <c r="B117" s="2">
         <v>5.01</v>
       </c>
-      <c r="E117" s="5">
+      <c r="E117" s="4">
         <f t="shared" si="3"/>
         <v>299.40119760479041</v>
       </c>
       <c r="H117" s="1"/>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A118" s="3" t="s">
+      <c r="A118" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B118" s="3">
+      <c r="B118" s="2">
         <v>5.63</v>
       </c>
-      <c r="E118" s="5">
+      <c r="E118" s="4">
         <f t="shared" si="3"/>
         <v>266.42984014209594</v>
       </c>
       <c r="H118" s="1"/>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
+      <c r="A119" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B119" s="3">
+      <c r="B119" s="2">
         <v>6.19</v>
       </c>
-      <c r="E119" s="5">
+      <c r="E119" s="4">
         <f t="shared" si="3"/>
         <v>242.32633279483036</v>
       </c>
       <c r="H119" s="1"/>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A120" s="3" t="s">
+      <c r="A120" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B120" s="3">
+      <c r="B120" s="2">
         <v>9.18</v>
       </c>
-      <c r="E120" s="5">
+      <c r="E120" s="4">
         <f t="shared" si="3"/>
         <v>163.39869281045753</v>
       </c>
       <c r="H120" s="1"/>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="3" t="s">
+      <c r="A121" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B121" s="3">
+      <c r="B121" s="2">
         <v>10.49</v>
       </c>
-      <c r="E121" s="5">
+      <c r="E121" s="4">
         <f t="shared" si="3"/>
         <v>142.99332697807435</v>
       </c>
       <c r="H121" s="1"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="s">
+      <c r="A122" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B122" s="3">
+      <c r="B122" s="2">
         <v>12.42</v>
       </c>
-      <c r="E122" s="5">
+      <c r="E122" s="4">
         <f t="shared" si="3"/>
         <v>120.77294685990339</v>
       </c>
       <c r="H122" s="1"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A123" s="3" t="s">
+      <c r="A123" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B123" s="3">
+      <c r="B123" s="2">
         <v>8.98</v>
       </c>
-      <c r="E123" s="5">
+      <c r="E123" s="4">
         <f>(1500+194963)/B123</f>
         <v>21877.839643652562</v>
       </c>
       <c r="H123" s="1"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
+      <c r="A124" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B124" s="3">
+      <c r="B124" s="2">
         <v>8.34</v>
       </c>
-      <c r="E124" s="5">
+      <c r="E124" s="4">
         <f t="shared" si="3"/>
         <v>179.85611510791367</v>
       </c>
       <c r="H124" s="1"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A125" s="3" t="s">
+      <c r="A125" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B125" s="3">
+      <c r="B125" s="2">
         <v>9.42</v>
       </c>
-      <c r="E125" s="5">
+      <c r="E125" s="4">
         <f t="shared" si="3"/>
         <v>159.23566878980893</v>
       </c>
       <c r="H125" s="1"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A126" s="3" t="s">
+      <c r="A126" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B126" s="3">
+      <c r="B126" s="2">
         <v>7.78</v>
       </c>
-      <c r="E126" s="5">
+      <c r="E126" s="4">
         <f t="shared" si="3"/>
         <v>192.80205655526993</v>
       </c>
       <c r="H126" s="1"/>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="3" t="s">
+      <c r="A127" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B127" s="3">
+      <c r="B127" s="2">
         <v>7.32</v>
       </c>
-      <c r="E127" s="5">
+      <c r="E127" s="4">
         <f t="shared" si="3"/>
         <v>204.91803278688525</v>
       </c>
       <c r="H127" s="1"/>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A128" s="3" t="s">
+      <c r="A128" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B128" s="3">
+      <c r="B128" s="2">
         <v>7.88</v>
       </c>
-      <c r="E128" s="5">
+      <c r="E128" s="4">
         <f t="shared" si="3"/>
         <v>190.35532994923858</v>
       </c>
       <c r="H128" s="1"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A129" s="3" t="s">
+      <c r="A129" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B129" s="3">
+      <c r="B129" s="2">
         <v>11.15</v>
       </c>
-      <c r="E129" s="5">
+      <c r="E129" s="4">
         <f t="shared" si="3"/>
         <v>134.52914798206277</v>
       </c>
       <c r="H129" s="1"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A130" s="3" t="s">
+      <c r="A130" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B130" s="3">
+      <c r="B130" s="2">
         <v>10.29</v>
       </c>
-      <c r="E130" s="5">
+      <c r="E130" s="4">
         <f t="shared" si="3"/>
         <v>145.77259475218659</v>
       </c>
       <c r="H130" s="1"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
+      <c r="A131" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B131" s="3">
+      <c r="B131" s="2">
         <v>11.7</v>
       </c>
-      <c r="E131" s="5">
+      <c r="E131" s="4">
         <f t="shared" si="3"/>
         <v>128.2051282051282</v>
       </c>
       <c r="H131" s="1"/>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A132" s="3" t="s">
+      <c r="A132" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B132" s="3">
+      <c r="B132" s="2">
         <v>11.47</v>
       </c>
-      <c r="E132" s="5">
+      <c r="E132" s="4">
         <f t="shared" si="3"/>
         <v>130.77593722755012</v>
       </c>
       <c r="H132" s="1"/>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A133" s="3" t="s">
+      <c r="A133" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B133" s="3">
+      <c r="B133" s="2">
         <v>11.26</v>
       </c>
-      <c r="E133" s="5">
+      <c r="E133" s="4">
         <f t="shared" si="3"/>
         <v>133.21492007104797</v>
       </c>
       <c r="H133" s="1"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A134" s="3" t="s">
+      <c r="A134" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B134" s="3">
+      <c r="B134" s="2">
         <v>9.86</v>
       </c>
-      <c r="E134" s="5">
+      <c r="E134" s="4">
         <f t="shared" si="3"/>
         <v>152.12981744421907</v>
       </c>
       <c r="H134" s="1"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A135" s="3" t="s">
+      <c r="A135" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B135" s="3">
+      <c r="B135" s="2">
         <v>8.68</v>
       </c>
-      <c r="E135" s="5">
+      <c r="E135" s="4">
         <f t="shared" si="3"/>
         <v>172.81105990783411</v>
       </c>
@@ -4289,12 +4395,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4303,90 +4410,90 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="33.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="32">
         <f>1500*360</f>
         <v>540000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="34"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="33"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B4" s="33">
         <v>3467322.27</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="34"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="33"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="33">
         <v>88051</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="33"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="B8" s="34">
+      <c r="B8" s="33">
         <v>271798</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>165</v>
       </c>
-      <c r="B10" s="34">
+      <c r="B10" s="33">
         <v>282701</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="29"/>
-      <c r="B11" s="27"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="26"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="B12" s="36">
+      <c r="B12" s="35">
         <f>SUM(B4:B10)</f>
         <v>4109872.27</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="28"/>
+      <c r="B13" s="27"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
+      <c r="B14" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>